<commit_message>
BMED Autoregressive model under developing
</commit_message>
<xml_diff>
--- a/Project/BMED/Data treatment/250110_BMED_train data_v1.xlsx
+++ b/Project/BMED/Data treatment/250110_BMED_train data_v1.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\bsjun\Documents\workspace\Git\repos_python\Project\BMED\Data treatment\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\USER\repos_python\Project\BMED\Data treatment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{78AA73D5-5BF6-4C50-AEBE-7F56D4D7EFED}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{247F6815-92E3-4A5D-BE8C-D9F9D2547DF4}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="14370" windowHeight="9150" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -4524,7 +4524,7 @@
       <selection activeCell="E117" sqref="E117"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" t="s">
@@ -7405,9 +7405,9 @@
       <selection pane="bottomLeft" sqref="A1:U281"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <cols>
-    <col min="11" max="11" width="28.08203125" bestFit="1" customWidth="1"/>
+    <col min="11" max="11" width="28.125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:21">
@@ -16288,7 +16288,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="131" spans="1:21" ht="17.5">
+    <row r="131" spans="1:21" ht="17.25">
       <c r="A131" s="49">
         <v>28.8</v>
       </c>
@@ -16357,7 +16357,7 @@
         <v>-8.2726137044532244E-2</v>
       </c>
     </row>
-    <row r="132" spans="1:21" ht="17.5">
+    <row r="132" spans="1:21" ht="17.25">
       <c r="A132" s="49">
         <v>22.3</v>
       </c>
@@ -16426,7 +16426,7 @@
         <v>2.3624749867161086</v>
       </c>
     </row>
-    <row r="133" spans="1:21" ht="17.5">
+    <row r="133" spans="1:21" ht="17.25">
       <c r="A133" s="49">
         <v>24.9</v>
       </c>
@@ -16495,7 +16495,7 @@
         <v>2.5963558532295594</v>
       </c>
     </row>
-    <row r="134" spans="1:21" ht="17.5">
+    <row r="134" spans="1:21" ht="17.25">
       <c r="A134" s="49">
         <v>26</v>
       </c>
@@ -16564,7 +16564,7 @@
         <v>3.8790774842491</v>
       </c>
     </row>
-    <row r="135" spans="1:21" ht="17.5">
+    <row r="135" spans="1:21" ht="17.25">
       <c r="A135" s="49">
         <v>26.4</v>
       </c>
@@ -16633,7 +16633,7 @@
         <v>4.703778594281709</v>
       </c>
     </row>
-    <row r="136" spans="1:21" ht="17.5">
+    <row r="136" spans="1:21" ht="17.25">
       <c r="A136" s="50">
         <v>26.2</v>
       </c>
@@ -16702,7 +16702,7 @@
         <v>5.2730137134975639</v>
       </c>
     </row>
-    <row r="137" spans="1:21" ht="17.5">
+    <row r="137" spans="1:21" ht="17.25">
       <c r="A137" s="50">
         <v>26</v>
       </c>
@@ -16771,7 +16771,7 @@
         <v>5.5793035284275261</v>
       </c>
     </row>
-    <row r="138" spans="1:21" ht="17.5">
+    <row r="138" spans="1:21" ht="17.25">
       <c r="A138" s="92">
         <v>22.7</v>
       </c>
@@ -16836,7 +16836,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="139" spans="1:21" ht="17.5">
+    <row r="139" spans="1:21" ht="17.25">
       <c r="A139" s="92">
         <v>23.7</v>
       </c>
@@ -16905,7 +16905,7 @@
         <v>0.42598812311885581</v>
       </c>
     </row>
-    <row r="140" spans="1:21" ht="17.5">
+    <row r="140" spans="1:21" ht="17.25">
       <c r="A140" s="92">
         <v>26.7</v>
       </c>
@@ -16974,7 +16974,7 @@
         <v>2.379399342078544</v>
       </c>
     </row>
-    <row r="141" spans="1:21" ht="17.5">
+    <row r="141" spans="1:21" ht="17.25">
       <c r="A141" s="92">
         <v>27.7</v>
       </c>
@@ -17043,7 +17043,7 @@
         <v>3.4908035395993808</v>
       </c>
     </row>
-    <row r="142" spans="1:21" ht="17.5">
+    <row r="142" spans="1:21" ht="17.25">
       <c r="A142" s="92">
         <v>28.4</v>
       </c>
@@ -17112,7 +17112,7 @@
         <v>4.4023149088250833</v>
       </c>
     </row>
-    <row r="143" spans="1:21" ht="17.5">
+    <row r="143" spans="1:21" ht="17.25">
       <c r="A143" s="92">
         <v>28.4</v>
       </c>
@@ -17181,7 +17181,7 @@
         <v>5.0344921523237085</v>
       </c>
     </row>
-    <row r="144" spans="1:21" ht="17.5">
+    <row r="144" spans="1:21" ht="17.25">
       <c r="A144" s="92">
         <v>28.2</v>
       </c>
@@ -17250,7 +17250,7 @@
         <v>5.5213124917082945</v>
       </c>
     </row>
-    <row r="145" spans="1:21" ht="17.5">
+    <row r="145" spans="1:21" ht="17.25">
       <c r="A145" s="102">
         <v>24.7</v>
       </c>
@@ -17315,7 +17315,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="146" spans="1:21" ht="17.5">
+    <row r="146" spans="1:21" ht="17.25">
       <c r="A146" s="78">
         <v>19.600000000000001</v>
       </c>
@@ -17384,7 +17384,7 @@
         <v>8.5216082880082977E-2</v>
       </c>
     </row>
-    <row r="147" spans="1:21" ht="17.5">
+    <row r="147" spans="1:21" ht="17.25">
       <c r="A147" s="78">
         <v>19.3</v>
       </c>
@@ -22308,7 +22308,7 @@
         <v>2.5237554898270136</v>
       </c>
     </row>
-    <row r="219" spans="1:21" ht="17.5">
+    <row r="219" spans="1:21" ht="17.25">
       <c r="A219" s="68">
         <v>18</v>
       </c>
@@ -22377,7 +22377,7 @@
         <v>2.8221452259311892</v>
       </c>
     </row>
-    <row r="220" spans="1:21" ht="17.5">
+    <row r="220" spans="1:21" ht="17.25">
       <c r="A220" s="104">
         <v>22.5</v>
       </c>
@@ -26761,7 +26761,7 @@
       <selection activeCell="L45" sqref="L45"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:9">
       <c r="A1" s="25" t="s">
@@ -26995,7 +26995,7 @@
         <v>543.99318984124682</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="17.5">
+    <row r="9" spans="1:9" ht="17.25">
       <c r="A9" s="49">
         <v>22.3</v>
       </c>
@@ -27459,7 +27459,7 @@
         <v>1337.4265428000001</v>
       </c>
     </row>
-    <row r="25" spans="1:9" ht="17.5">
+    <row r="25" spans="1:9" ht="17.25">
       <c r="A25" s="49">
         <v>28.8</v>
       </c>
@@ -27546,7 +27546,7 @@
         <v>60.420076255709098</v>
       </c>
     </row>
-    <row r="28" spans="1:9" ht="17.5">
+    <row r="28" spans="1:9" ht="17.25">
       <c r="A28" s="49">
         <v>24.9</v>
       </c>
@@ -28474,7 +28474,7 @@
         <v>222.06601934981819</v>
       </c>
     </row>
-    <row r="60" spans="1:9" ht="17.5">
+    <row r="60" spans="1:9" ht="17.25">
       <c r="A60" s="85">
         <v>26</v>
       </c>
@@ -29750,7 +29750,7 @@
         <v>61.525458909090922</v>
       </c>
     </row>
-    <row r="104" spans="1:9" ht="17.5">
+    <row r="104" spans="1:9" ht="17.25">
       <c r="A104" s="49">
         <v>26.4</v>
       </c>
@@ -30069,7 +30069,7 @@
         <v>349.62176099054534</v>
       </c>
     </row>
-    <row r="115" spans="1:9" ht="17.5">
+    <row r="115" spans="1:9" ht="17.25">
       <c r="A115" s="68">
         <v>18</v>
       </c>
@@ -30881,7 +30881,7 @@
         <v>199.96386116218187</v>
       </c>
     </row>
-    <row r="143" spans="1:9" ht="17.5">
+    <row r="143" spans="1:9" ht="17.25">
       <c r="A143" s="50">
         <v>26.2</v>
       </c>
@@ -31809,7 +31809,7 @@
         <v>333.00426019694538</v>
       </c>
     </row>
-    <row r="175" spans="1:9" ht="17.5">
+    <row r="175" spans="1:9" ht="17.25">
       <c r="A175" s="50">
         <v>26</v>
       </c>
@@ -32186,7 +32186,7 @@
         <v>617.25194930908924</v>
       </c>
     </row>
-    <row r="188" spans="1:9" ht="17.5">
+    <row r="188" spans="1:9" ht="17.25">
       <c r="A188" s="29">
         <v>25.7</v>
       </c>
@@ -33013,10 +33013,10 @@
   <dimension ref="A1:W216"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J2" sqref="J2"/>
+      <selection activeCell="U4" sqref="U4"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="17"/>
+  <sheetFormatPr defaultRowHeight="16.5"/>
   <sheetData>
     <row r="1" spans="1:23">
       <c r="A1" t="s">
@@ -33149,7 +33149,6 @@
         <v>0</v>
       </c>
       <c r="U2" s="106">
-        <f>F2*M2/$M$2*P2</f>
         <v>1</v>
       </c>
       <c r="V2" s="106">
@@ -33225,11 +33224,11 @@
         <v>8.3434664986866691E-3</v>
       </c>
       <c r="U3" s="106">
-        <f t="shared" ref="U3:U7" si="1">F3*M3/$M$2*P3</f>
+        <f>F3*M3/$M$2*P3</f>
         <v>1.012353376365442</v>
       </c>
       <c r="V3" s="106">
-        <f t="shared" ref="V3:V57" si="2">F3-U3</f>
+        <f t="shared" ref="V3:V57" si="1">F3-U3</f>
         <v>-1.2353376365441981E-2</v>
       </c>
       <c r="W3">
@@ -33293,7 +33292,7 @@
         <v>0.98</v>
       </c>
       <c r="S4" s="106">
-        <f t="shared" ref="S3:S7" si="3">E4*J4/$J$2*P4</f>
+        <f t="shared" ref="S4:S7" si="2">E4*J4/$J$2*P4</f>
         <v>0.46336443859741527</v>
       </c>
       <c r="T4" s="106">
@@ -33301,11 +33300,11 @@
         <v>3.6635561402584726E-2</v>
       </c>
       <c r="U4" s="106">
+        <f t="shared" ref="U3:U7" si="3">F4*M4/$M$2*P4</f>
+        <v>0.82680587002096451</v>
+      </c>
+      <c r="V4" s="106">
         <f t="shared" si="1"/>
-        <v>0.82680587002096451</v>
-      </c>
-      <c r="V4" s="106">
-        <f t="shared" si="2"/>
         <v>0.17319412997903549</v>
       </c>
       <c r="W4">
@@ -33369,7 +33368,7 @@
         <v>1.01</v>
       </c>
       <c r="S5" s="106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.39578062255181923</v>
       </c>
       <c r="T5" s="106">
@@ -33377,11 +33376,11 @@
         <v>0.10421937744818077</v>
       </c>
       <c r="U5" s="106">
+        <f t="shared" si="3"/>
+        <v>0.58051463770274736</v>
+      </c>
+      <c r="V5" s="106">
         <f t="shared" si="1"/>
-        <v>0.58051463770274736</v>
-      </c>
-      <c r="V5" s="106">
-        <f t="shared" si="2"/>
         <v>0.41948536229725264</v>
       </c>
       <c r="W5">
@@ -33445,7 +33444,7 @@
         <v>1.02</v>
       </c>
       <c r="S6" s="106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.27708197714579641</v>
       </c>
       <c r="T6" s="106">
@@ -33453,11 +33452,11 @@
         <v>0.22291802285420359</v>
       </c>
       <c r="U6" s="106">
+        <f t="shared" si="3"/>
+        <v>0.34926810669756148</v>
+      </c>
+      <c r="V6" s="106">
         <f t="shared" si="1"/>
-        <v>0.34926810669756148</v>
-      </c>
-      <c r="V6" s="106">
-        <f t="shared" si="2"/>
         <v>0.65073189330243852</v>
       </c>
       <c r="W6">
@@ -33521,7 +33520,7 @@
         <v>1.1200000000000001</v>
       </c>
       <c r="S7" s="106">
-        <f t="shared" si="3"/>
+        <f t="shared" si="2"/>
         <v>0.10177861466651056</v>
       </c>
       <c r="T7" s="106">
@@ -33529,11 +33528,11 @@
         <v>0.39822138533348944</v>
       </c>
       <c r="U7" s="106">
+        <f t="shared" si="3"/>
+        <v>0.2014704187722976</v>
+      </c>
+      <c r="V7" s="106">
         <f t="shared" si="1"/>
-        <v>0.2014704187722976</v>
-      </c>
-      <c r="V7" s="106">
-        <f t="shared" si="2"/>
         <v>0.79852958122770246</v>
       </c>
       <c r="W7">
@@ -33605,7 +33604,7 @@
         <v>1</v>
       </c>
       <c r="V8" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W8">
@@ -33681,7 +33680,7 @@
         <v>0.99586692144333788</v>
       </c>
       <c r="V9" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>4.1330785566621175E-3</v>
       </c>
       <c r="W9">
@@ -33757,7 +33756,7 @@
         <v>1.087107471975348</v>
       </c>
       <c r="V10" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-8.7107471975347961E-2</v>
       </c>
       <c r="W10">
@@ -33833,7 +33832,7 @@
         <v>0.99177366739124617</v>
       </c>
       <c r="V11" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>8.226332608753828E-3</v>
       </c>
       <c r="W11">
@@ -33909,7 +33908,7 @@
         <v>0.93178349342948485</v>
       </c>
       <c r="V12" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.8216506570515145E-2</v>
       </c>
       <c r="W12">
@@ -33985,7 +33984,7 @@
         <v>0.29929211369956682</v>
       </c>
       <c r="V13" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.70070788630043324</v>
       </c>
       <c r="W13">
@@ -34061,7 +34060,7 @@
         <v>0.27379815173453143</v>
       </c>
       <c r="V14" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.72620184826546863</v>
       </c>
       <c r="W14">
@@ -34209,7 +34208,7 @@
         <v>1</v>
       </c>
       <c r="V16" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W16">
@@ -34285,7 +34284,7 @@
         <v>0.99931160406536035</v>
       </c>
       <c r="V17" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>6.8839593463965176E-4</v>
       </c>
       <c r="W17">
@@ -34361,7 +34360,7 @@
         <v>0.57651938219972887</v>
       </c>
       <c r="V18" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.42348061780027113</v>
       </c>
       <c r="W18">
@@ -34437,7 +34436,7 @@
         <v>0.33219163628176135</v>
       </c>
       <c r="V19" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.6678083637182386</v>
       </c>
       <c r="W19">
@@ -34513,7 +34512,7 @@
         <v>0.18606054980716089</v>
       </c>
       <c r="V20" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.81393945019283909</v>
       </c>
       <c r="W20">
@@ -34589,7 +34588,7 @@
         <v>3.3306375957334548E-3</v>
       </c>
       <c r="V21" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.99666936240426651</v>
       </c>
       <c r="W21">
@@ -34661,7 +34660,7 @@
         <v>2</v>
       </c>
       <c r="V22" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W22">
@@ -34737,7 +34736,7 @@
         <v>1.6603645830648277</v>
       </c>
       <c r="V23" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.3396354169351723</v>
       </c>
       <c r="W23">
@@ -34813,7 +34812,7 @@
         <v>1.3913232117540919</v>
       </c>
       <c r="V24" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.6086767882459081</v>
       </c>
       <c r="W24">
@@ -34889,7 +34888,7 @@
         <v>6.9495858299265375E-3</v>
       </c>
       <c r="V25" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9930504141700736</v>
       </c>
       <c r="W25">
@@ -34965,7 +34964,7 @@
         <v>2.9941503901018177E-3</v>
       </c>
       <c r="V26" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9970058496098981</v>
       </c>
       <c r="W26">
@@ -35037,7 +35036,7 @@
         <v>2</v>
       </c>
       <c r="V27" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W27" s="109">
@@ -35113,7 +35112,7 @@
         <v>1.7573086194181811</v>
       </c>
       <c r="V28" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.24269138058181894</v>
       </c>
       <c r="W28">
@@ -35189,7 +35188,7 @@
         <v>1.6091298306054833</v>
       </c>
       <c r="V29" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.39087016939451669</v>
       </c>
       <c r="W29">
@@ -35265,7 +35264,7 @@
         <v>1.1421919611900542</v>
       </c>
       <c r="V30" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.85780803880994583</v>
       </c>
       <c r="W30">
@@ -35341,7 +35340,7 @@
         <v>0.66211418445180659</v>
       </c>
       <c r="V31" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.3378858155481934</v>
       </c>
       <c r="W31">
@@ -35417,7 +35416,7 @@
         <v>2.9422159252668516E-3</v>
       </c>
       <c r="V32" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9970577840747332</v>
       </c>
       <c r="W32">
@@ -35489,7 +35488,7 @@
         <v>2</v>
       </c>
       <c r="V33" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W33" s="109">
@@ -35565,7 +35564,7 @@
         <v>1.7825883099976125</v>
       </c>
       <c r="V34" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.21741169000238747</v>
       </c>
       <c r="W34">
@@ -35641,7 +35640,7 @@
         <v>1.3369466654582298</v>
       </c>
       <c r="V35" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.66305333454177018</v>
       </c>
       <c r="W35">
@@ -35717,7 +35716,7 @@
         <v>0.86907737218693792</v>
       </c>
       <c r="V36" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.130922627813062</v>
       </c>
       <c r="W36">
@@ -35793,7 +35792,7 @@
         <v>0.57057971074692637</v>
       </c>
       <c r="V37" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.4294202892530736</v>
       </c>
       <c r="W37">
@@ -35869,7 +35868,7 @@
         <v>0.33846928228125861</v>
       </c>
       <c r="V38" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.6615307177187413</v>
       </c>
       <c r="W38">
@@ -35945,7 +35944,7 @@
         <v>0.19642949542785082</v>
       </c>
       <c r="V39" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8035705045721491</v>
       </c>
       <c r="W39">
@@ -36021,7 +36020,7 @@
         <v>2.6911676014617541E-3</v>
       </c>
       <c r="V40" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.9973088323985382</v>
       </c>
       <c r="W40">
@@ -36093,7 +36092,7 @@
         <v>1</v>
       </c>
       <c r="V41" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W41" s="109">
@@ -36169,7 +36168,7 @@
         <v>0.97272709045517847</v>
       </c>
       <c r="V42" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>2.7272909544821533E-2</v>
       </c>
       <c r="W42">
@@ -36245,7 +36244,7 @@
         <v>0.67800390010585376</v>
       </c>
       <c r="V43" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.32199609989414624</v>
       </c>
       <c r="W43">
@@ -36321,7 +36320,7 @@
         <v>0.36696417480090626</v>
       </c>
       <c r="V44" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.63303582519909374</v>
       </c>
       <c r="W44">
@@ -36397,7 +36396,7 @@
         <v>7.6390497360260667E-3</v>
       </c>
       <c r="V45" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.99236095026397397</v>
       </c>
       <c r="W45">
@@ -36469,7 +36468,7 @@
         <v>2</v>
       </c>
       <c r="V46" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W46" s="109">
@@ -36545,7 +36544,7 @@
         <v>1.8163487284106026</v>
       </c>
       <c r="V47" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.18365127158939742</v>
       </c>
       <c r="W47">
@@ -36621,7 +36620,7 @@
         <v>1.3589318079141641</v>
       </c>
       <c r="V48" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.64106819208583588</v>
       </c>
       <c r="W48">
@@ -36697,7 +36696,7 @@
         <v>0.98488315475809129</v>
       </c>
       <c r="V49" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.0151168452419088</v>
       </c>
       <c r="W49">
@@ -36773,7 +36772,7 @@
         <v>0.44220735260470517</v>
       </c>
       <c r="V50" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.5577926473952948</v>
       </c>
       <c r="W50">
@@ -36849,7 +36848,7 @@
         <v>0.15301356797056542</v>
       </c>
       <c r="V51" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>1.8469864320294347</v>
       </c>
       <c r="W51">
@@ -36921,7 +36920,7 @@
         <v>1.5</v>
       </c>
       <c r="V52" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0</v>
       </c>
       <c r="W52" s="109">
@@ -36997,7 +36996,7 @@
         <v>1.5192218236047421</v>
       </c>
       <c r="V53" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>-1.9221823604742116E-2</v>
       </c>
       <c r="W53">
@@ -37073,7 +37072,7 @@
         <v>1.2632142077116</v>
       </c>
       <c r="V54" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.23678579228840002</v>
       </c>
       <c r="W54">
@@ -37149,7 +37148,7 @@
         <v>1.0812238111757477</v>
       </c>
       <c r="V55" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.41877618882425227</v>
       </c>
       <c r="W55">
@@ -37225,7 +37224,7 @@
         <v>0.91131604089539964</v>
       </c>
       <c r="V56" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.58868395910460036</v>
       </c>
       <c r="W56">
@@ -37301,7 +37300,7 @@
         <v>0.65358528980508324</v>
       </c>
       <c r="V57" s="106">
-        <f t="shared" si="2"/>
+        <f t="shared" si="1"/>
         <v>0.84641471019491676</v>
       </c>
       <c r="W57">
@@ -40397,7 +40396,7 @@
         <v>24.485714285714288</v>
       </c>
     </row>
-    <row r="99" spans="1:23" ht="17.5">
+    <row r="99" spans="1:23" ht="17.25">
       <c r="A99">
         <v>16</v>
       </c>
@@ -40469,7 +40468,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="100" spans="1:23" ht="17.5">
+    <row r="100" spans="1:23" ht="17.25">
       <c r="A100">
         <v>16</v>
       </c>
@@ -40545,7 +40544,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="101" spans="1:23" ht="17.5">
+    <row r="101" spans="1:23" ht="17.25">
       <c r="A101">
         <v>16</v>
       </c>
@@ -40621,7 +40620,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="102" spans="1:23" ht="17.5">
+    <row r="102" spans="1:23" ht="17.25">
       <c r="A102">
         <v>16</v>
       </c>
@@ -40697,7 +40696,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="103" spans="1:23" ht="17.5">
+    <row r="103" spans="1:23" ht="17.25">
       <c r="A103">
         <v>16</v>
       </c>
@@ -40773,7 +40772,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="104" spans="1:23" ht="17.5">
+    <row r="104" spans="1:23" ht="17.25">
       <c r="A104">
         <v>16</v>
       </c>
@@ -40849,7 +40848,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="105" spans="1:23" ht="17.5">
+    <row r="105" spans="1:23" ht="17.25">
       <c r="A105">
         <v>16</v>
       </c>
@@ -40925,7 +40924,7 @@
         <v>26.542857142857141</v>
       </c>
     </row>
-    <row r="106" spans="1:23" ht="17.5">
+    <row r="106" spans="1:23" ht="17.25">
       <c r="A106">
         <v>17</v>
       </c>
@@ -40997,7 +40996,7 @@
         <v>20.839999999999996</v>
       </c>
     </row>
-    <row r="107" spans="1:23" ht="17.5">
+    <row r="107" spans="1:23" ht="17.25">
       <c r="A107">
         <v>17</v>
       </c>
@@ -41073,7 +41072,7 @@
         <v>20.839999999999996</v>
       </c>
     </row>
-    <row r="108" spans="1:23" ht="17.5">
+    <row r="108" spans="1:23" ht="17.25">
       <c r="A108">
         <v>17</v>
       </c>
@@ -45521,7 +45520,7 @@
         <v>19.400000000000002</v>
       </c>
     </row>
-    <row r="167" spans="1:23" ht="17.5">
+    <row r="167" spans="1:23" ht="17.25">
       <c r="A167">
         <v>27</v>
       </c>

</xml_diff>